<commit_message>
Join en Create menu aanmaken + button working
</commit_message>
<xml_diff>
--- a/doc/schema_s/DatabaseModel1.xlsx
+++ b/doc/schema_s/DatabaseModel1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Documents\School1819\CA1819-Taken5BartEdition\doc\schema_s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B091ADFE-C801-40D5-A52A-7CB0F4E86BFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C532EB-AFFF-432A-AD72-AEA5E2F67EAB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{3CD7DFD1-C994-498A-819C-0428C3AEBA03}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Game</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>positie in ranglijst</t>
+  </si>
+  <si>
+    <t>naam</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <dimension ref="A4:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,11 +546,17 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>

</xml_diff>